<commit_message>
optimized generating session table
</commit_message>
<xml_diff>
--- a/data/regions.xlsx
+++ b/data/regions.xlsx
@@ -86,181 +86,181 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>50.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Неизвестный</t>
+          <t>Республика Дагестан</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>51.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Белгород</t>
+          <t>Республика Ингушетия</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>41.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ставропольский край</t>
+          <t>Карачаево-Черкесская Республика</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>38.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Свердловская область</t>
+          <t>Астраханская область</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>18.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Международный</t>
+          <t>Москва</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>35.0</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Тамбовская область</t>
+          <t>Омская область</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>34.0</v>
+        <v>7.0</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Челябинская область</t>
+          <t>Краснодарский край</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>33.0</v>
+        <v>8.0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Калининградская область</t>
+          <t>Киргизия</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>32.0</v>
+        <v>9.0</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Воронежская область</t>
+          <t>Абхазия</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>31.0</v>
+        <v>10.0</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Красноярский край</t>
+          <t>Ульяновская область</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>30.0</v>
+        <v>11.0</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Хабаровский край</t>
+          <t>Чеченская Республика</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>29.0</v>
+        <v>13.0</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Московская область</t>
+          <t>Санкт-Петербург</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>28.0</v>
+        <v>14.0</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Кемеровская область</t>
+          <t>Костромская область</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>27.0</v>
+        <v>15.0</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Республика Мордовия</t>
+          <t>Республика Башкортостан</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>26.0</v>
+        <v>16.0</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ярославская область</t>
+          <t>Пермский край</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>25.0</v>
+        <v>17.0</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Приморский край</t>
+          <t>Республика Татарстан</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>24.0</v>
+        <v>18.0</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Чувашская Республика</t>
+          <t>Международный</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Новосибирская область</t>
+          <t>Иркутск</t>
         </is>
       </c>
     </row>
@@ -276,211 +276,211 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>17.0</v>
+        <v>22.0</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Республика Татарстан</t>
+          <t>Новосибирская область</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>16.0</v>
+        <v>24.0</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Пермский край</t>
+          <t>Чувашская Республика</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>15.0</v>
+        <v>25.0</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Республика Башкортостан</t>
+          <t>Приморский край</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>14.0</v>
+        <v>26.0</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Костромская область</t>
+          <t>Ярославская область</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>13.0</v>
+        <v>27.0</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Санкт-Петербург</t>
+          <t>Республика Мордовия</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>11.0</v>
+        <v>28.0</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Чеченская Республика</t>
+          <t>Кемеровская область</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>10.0</v>
+        <v>29.0</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ульяновская область</t>
+          <t>Московская область</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>9.0</v>
+        <v>30.0</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Абхазия</t>
+          <t>Хабаровский край</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>8.0</v>
+        <v>31.0</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Киргизия</t>
+          <t>Красноярский край</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>7.0</v>
+        <v>32.0</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Краснодарский край</t>
+          <t>Воронежская область</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>6.0</v>
+        <v>33.0</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Омская область</t>
+          <t>Калининградская область</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>5.0</v>
+        <v>34.0</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Москва</t>
+          <t>Челябинская область</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>4.0</v>
+        <v>35.0</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Астраханская область</t>
+          <t>Тамбовская область</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>3.0</v>
+        <v>38.0</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Карачаево-Черкесская Республика</t>
+          <t>Свердловская область</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>2.0</v>
+        <v>40.0</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Республика Ингушетия</t>
+          <t>Пенза</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>1.0</v>
+        <v>41.0</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Республика Дагестан</t>
+          <t>Ставропольский край</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>20.0</v>
+        <v>45.0</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Иркутск</t>
+          <t>Республика Адыгея</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>40.0</v>
+        <v>46.0</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Пенза</t>
+          <t>Томск</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>45.0</v>
+        <v>47.0</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Республика Адыгея</t>
+          <t>Пермь</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>46.0</v>
+        <v>50.0</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Томск</t>
+          <t>Неизвестный</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>47.0</v>
+        <v>51.0</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Пермь</t>
+          <t>Белгород</t>
         </is>
       </c>
     </row>

</xml_diff>